<commit_message>
Changes to visualising distances.
</commit_message>
<xml_diff>
--- a/distance.xlsx
+++ b/distance.xlsx
@@ -500,31 +500,31 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8247863153616588</v>
+        <v>0.9029038349787394</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9310674965381622</v>
+        <v>0.9167482256889343</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7947156727313995</v>
+        <v>0.8286526948213577</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9119508564472198</v>
+        <v>0.8402521014213562</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7951687276363373</v>
+        <v>0.8015593141317368</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9571075439453125</v>
+        <v>0.9777853488922119</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9917326867580414</v>
+        <v>0.9856123328208923</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7863345146179199</v>
+        <v>0.7952601909637451</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8970734179019928</v>
+        <v>0.9316011667251587</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +534,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8796288371086121</v>
+        <v>0.8623180290063223</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.827721893787384</v>
+        <v>0.756869912147522</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8261846601963043</v>
+        <v>0.830847313006719</v>
       </c>
       <c r="F3" t="n">
-        <v>0.786892811457316</v>
+        <v>0.8537154396375021</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7450005114078522</v>
+        <v>0.8012186884880066</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9504347046216329</v>
+        <v>0.9441962639490763</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9861092070738474</v>
+        <v>0.9852280616760254</v>
       </c>
       <c r="J3" t="n">
-        <v>0.693064272403717</v>
+        <v>0.7365642786026001</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9602324763933817</v>
+        <v>0.9521704117457072</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +571,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9198962152004242</v>
+        <v>0.9504640698432922</v>
       </c>
       <c r="C4" t="n">
-        <v>0.800685981909434</v>
+        <v>0.8124158382415771</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9440264999866486</v>
+        <v>0.9371106326580048</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9838683009147644</v>
+        <v>0.9950271844863892</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9541944563388824</v>
+        <v>0.9532506465911865</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9808092713356018</v>
+        <v>0.95600825548172</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9930621683597565</v>
+        <v>0.9846462905406952</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9761677384376526</v>
+        <v>0.9648858904838562</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9206585288047791</v>
+        <v>0.9573302268981934</v>
       </c>
     </row>
     <row r="5">
@@ -608,34 +608,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8144536912441254</v>
+        <v>0.8235698044300079</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7721575895945232</v>
+        <v>0.821491003036499</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9306925237178802</v>
+        <v>0.9481375217437744</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.939351886510849</v>
+        <v>0.9241468608379364</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8037624210119247</v>
+        <v>0.8520738482475281</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9123736023902893</v>
+        <v>0.9246824085712433</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9272354394197464</v>
+        <v>0.9620617628097534</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8840766549110413</v>
+        <v>0.9240339994430542</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8745200634002686</v>
+        <v>0.8459548950195312</v>
       </c>
     </row>
     <row r="6">
@@ -645,34 +645,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9042466580867767</v>
+        <v>0.8665298223495483</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8524986505508423</v>
+        <v>0.7938462098439535</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9961380362510681</v>
+        <v>0.9981905817985535</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9267493784427643</v>
+        <v>0.9416531324386597</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.967390775680542</v>
+        <v>0.9633549749851227</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9586446285247803</v>
+        <v>0.9462270736694336</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9752399623394012</v>
+        <v>0.9797036647796631</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9352759122848511</v>
+        <v>0.9467079043388367</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9711480140686035</v>
+        <v>0.9381299614906311</v>
       </c>
     </row>
     <row r="7">
@@ -682,34 +682,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8027789443731308</v>
+        <v>0.8539272546768188</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7767466704050699</v>
+        <v>0.8183208306630453</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9301902055740356</v>
+        <v>0.9335795938968658</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8017322272062302</v>
+        <v>0.8379693478345871</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9428035020828247</v>
+        <v>0.9150501489639282</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9474880397319794</v>
+        <v>0.9320261478424072</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9714255183935165</v>
+        <v>0.9759467393159866</v>
       </c>
       <c r="J7" t="n">
-        <v>0.862675666809082</v>
+        <v>0.865458756685257</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8579877018928528</v>
+        <v>0.8839512765407562</v>
       </c>
     </row>
     <row r="8">
@@ -719,34 +719,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9766134917736053</v>
+        <v>0.973026305437088</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9137768149375916</v>
+        <v>0.9541288812955221</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9448748230934143</v>
+        <v>0.9361419677734375</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9260894954204559</v>
+        <v>0.9305903613567352</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9812248349189758</v>
+        <v>0.9607416987419128</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9131119251251221</v>
+        <v>0.9218071103096008</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9987543821334839</v>
+        <v>0.9983170628547668</v>
       </c>
       <c r="J8" t="n">
-        <v>0.7788676619529724</v>
+        <v>0.7977302670478821</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9657214879989624</v>
+        <v>0.9633198976516724</v>
       </c>
     </row>
     <row r="9">
@@ -756,34 +756,34 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9952344447374344</v>
+        <v>0.9920817166566849</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9860035975774128</v>
+        <v>0.9894202649593353</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9899357259273529</v>
+        <v>0.9839665591716766</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9566459208726883</v>
+        <v>0.9576843231916428</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9821140468120575</v>
+        <v>0.9884465038776398</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9688922613859177</v>
+        <v>0.9761862307786942</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9985096752643585</v>
+        <v>0.9986096322536469</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9655601978302002</v>
+        <v>0.9546948075294495</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9958871603012085</v>
+        <v>0.9956967830657959</v>
       </c>
     </row>
     <row r="10">
@@ -793,34 +793,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8500657081604004</v>
+        <v>0.8155481219291687</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6951122681299845</v>
+        <v>0.6833437085151672</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9788686633110046</v>
+        <v>0.9411723613739014</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8575575053691864</v>
+        <v>0.8764290809631348</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9452908039093018</v>
+        <v>0.9361354112625122</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8412518203258514</v>
+        <v>0.902280867099762</v>
       </c>
       <c r="H10" t="n">
-        <v>0.8483715057373047</v>
+        <v>0.8584713935852051</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9757921695709229</v>
+        <v>0.9764431118965149</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8716192841529846</v>
+        <v>0.8363800644874573</v>
       </c>
     </row>
     <row r="11">
@@ -830,31 +830,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8059435784816742</v>
+        <v>0.8516279458999634</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9395831624666849</v>
+        <v>0.9452718098958334</v>
       </c>
       <c r="D11" t="n">
-        <v>0.908220648765564</v>
+        <v>0.9540036916732788</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8187345564365387</v>
+        <v>0.7847095429897308</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9555029273033142</v>
+        <v>0.9205443859100342</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8476782739162445</v>
+        <v>0.8490531444549561</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9681094884872437</v>
+        <v>0.95635986328125</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9984377026557922</v>
+        <v>0.9979508817195892</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8471822738647461</v>
+        <v>0.766191840171814</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>

</xml_diff>